<commit_message>
Changes mostly related to avoiding excess power consumption.  This is mainly by limiting the signal swing to 0..5V and using asymmetric supplies of -4V and +8V.  (Perhaps we can reduce these to 3/7 V.)  Also, I got rid of two stages in the input signal path.
power_budget.xlsx
power.sch
reference_buffer.sch:
Changes related to the new supply voltages, and start on the power supply section.

input_channel.sch
in_amp.sch
antialias_driver.sch:
Reworked the input signal chain to keep a full differential path, rolling the antialias filter
into the ADC driver.  Also, related to change to lower asymmetrical supply voltages, there is
no 20V PP anywhere (the this was for benefit of the antialias filter noise, but that stage is gone).  Also, added zener clamp on VREF in driver.

in_filter.sch: added missing DC bias resistors.
</commit_message>
<xml_diff>
--- a/input/power_budget.xlsx
+++ b/input/power_budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_hw\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C47B020-2092-4E8E-8852-0B5313AE4136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD33C5AC-2883-4456-A7A1-C15931A2A4CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="705" windowWidth="19425" windowHeight="10890" activeTab="2" xr2:uid="{A167505A-04D4-416C-9B79-616B1C61F63E}"/>
+    <workbookView xWindow="420" yWindow="1380" windowWidth="19425" windowHeight="10890" activeTab="2" xr2:uid="{A167505A-04D4-416C-9B79-616B1C61F63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan A" sheetId="1" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="K1" sqref="K1:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mostly start of work on the lv_regs project for the low-voltage regulator daughtercard to the main board. Also made a directory with the revision 0 main board output files. Where the files are located, and what kicad libraries components are in is kind of a mess.
</commit_message>
<xml_diff>
--- a/input/power_budget.xlsx
+++ b/input/power_budget.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_hw\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A1EF38-3CF1-4E4B-9142-EACF488D0A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39FA60-A4FC-43A9-B6CC-9D031421B02E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1224" yWindow="1164" windowWidth="19548" windowHeight="10572" activeTab="2" xr2:uid="{A167505A-04D4-416C-9B79-616B1C61F63E}"/>
-    <workbookView xWindow="1224" yWindow="11844" windowWidth="19644" windowHeight="11436" activeTab="1" xr2:uid="{98C7A632-B63B-4F5F-A047-55BAAA097B0D}"/>
+    <workbookView xWindow="11040" yWindow="6672" windowWidth="15372" windowHeight="16248" activeTab="2" xr2:uid="{A167505A-04D4-416C-9B79-616B1C61F63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input board" sheetId="4" r:id="rId1"/>
@@ -19,7 +18,6 @@
     <sheet name="Input carryover" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -488,60 +486,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,6 +510,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,7 +885,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -899,30 +896,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="K1" s="33" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="K1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="14" t="s">
         <v>21</v>
       </c>
@@ -932,13 +929,13 @@
       <c r="I2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -959,18 +956,18 @@
       <c r="F3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -991,13 +988,13 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1030,13 +1027,13 @@
         <f>I9/F5*1000</f>
         <v>10.494752623688155</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
     </row>
     <row r="6" spans="1:17" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1063,21 +1060,21 @@
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="6">
         <f>C4</f>
         <v>16</v>
@@ -1103,22 +1100,22 @@
         <f>SUM(I5:I6)</f>
         <v>60.494752623688157</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
     </row>
     <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F9" s="3" t="s">
@@ -1135,44 +1132,44 @@
       <c r="I9" s="5">
         <v>7</v>
       </c>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
     </row>
     <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1190,13 +1187,13 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1254,10 +1251,10 @@
       <c r="Q15" s="27"/>
     </row>
     <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="8">
         <f>C7*3+SUM(C12:C14)</f>
         <v>48</v>
@@ -1288,10 +1285,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="13">
         <f>C16/1000*C19</f>
         <v>0.24</v>
@@ -1320,10 +1317,10 @@
         <f>I16/1000*I19+SUM(C17:F17)</f>
         <v>4.7455481259370318</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="44"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
@@ -1390,9 +1387,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="1">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1404,23 +1398,23 @@
   </cols>
   <sheetData>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="38" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1461,16 +1455,16 @@
       <c r="A20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="34">
         <f>'Input carryover'!G9</f>
         <v>114.60000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="51">
+      <c r="B21" s="35">
         <f>SUM(B16:B20)</f>
         <v>1658.6</v>
       </c>
@@ -1488,10 +1482,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,57 +1491,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="44" t="s">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="47"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="48" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="41"/>
       <c r="C4">
         <f>'Input board'!C16</f>
         <v>48</v>
@@ -1567,50 +1558,50 @@
         <f>'Input board'!F16</f>
         <v>11</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="28">
         <f>'Input board'!E16+'Input board'!G16</f>
         <v>94.037347778852691</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="28">
         <f>'Input board'!E16+'Input board'!I16</f>
         <v>262.78425787106448</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="F6" s="41" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="F6" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="30" t="s">
         <v>37</v>
       </c>
       <c r="B8">
@@ -1624,21 +1615,21 @@
         <f>C8</f>
         <v>48</v>
       </c>
-      <c r="F8" s="38">
-        <f>C8*3</f>
+      <c r="F8" s="28">
+        <f t="shared" ref="F8:G11" si="0">C8*3</f>
         <v>144</v>
       </c>
-      <c r="G8" s="38">
-        <f>D8*3</f>
+      <c r="G8" s="28">
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
-      <c r="I8" s="49">
+      <c r="I8" s="33">
         <f>F8+F9</f>
         <v>258.60000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="30" t="s">
         <v>38</v>
       </c>
       <c r="B9">
@@ -1652,12 +1643,12 @@
         <f>C9</f>
         <v>38.200000000000003</v>
       </c>
-      <c r="F9" s="38">
-        <f>C9*3</f>
+      <c r="F9" s="28">
+        <f t="shared" si="0"/>
         <v>114.60000000000001</v>
       </c>
-      <c r="G9" s="38">
-        <f>D9*3</f>
+      <c r="G9" s="28">
+        <f t="shared" si="0"/>
         <v>114.60000000000001</v>
       </c>
     </row>
@@ -1668,20 +1659,20 @@
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="28">
         <f>G4+F4</f>
         <v>105.03734777885269</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="28">
         <f>H4+F4</f>
         <v>273.78425787106448</v>
       </c>
-      <c r="F10" s="38">
-        <f>C10*3</f>
+      <c r="F10" s="28">
+        <f t="shared" si="0"/>
         <v>315.11204333655809</v>
       </c>
-      <c r="G10" s="38">
-        <f>D10*3</f>
+      <c r="G10" s="28">
+        <f t="shared" si="0"/>
         <v>821.35277361319345</v>
       </c>
     </row>
@@ -1692,20 +1683,20 @@
       <c r="B11">
         <v>6</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="28">
         <f>G4</f>
         <v>94.037347778852691</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="28">
         <f>H4</f>
         <v>262.78425787106448</v>
       </c>
-      <c r="F11" s="38">
-        <f>C11*3</f>
+      <c r="F11" s="28">
+        <f t="shared" si="0"/>
         <v>282.11204333655809</v>
       </c>
-      <c r="G11" s="38">
-        <f>D11*3</f>
+      <c r="G11" s="28">
+        <f t="shared" si="0"/>
         <v>788.35277361319345</v>
       </c>
     </row>

</xml_diff>